<commit_message>
output - trained on gpu
</commit_message>
<xml_diff>
--- a/output/output_bert.xlsx
+++ b/output/output_bert.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -395,7 +395,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -635,7 +635,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -655,7 +655,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93">
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
@@ -1345,7 +1345,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -1415,7 +1415,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
@@ -1865,7 +1865,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -1895,7 +1895,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -2015,7 +2015,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -2235,7 +2235,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
@@ -2365,7 +2365,7 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -2405,7 +2405,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205">
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="209">
@@ -2455,7 +2455,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
@@ -2525,7 +2525,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="217">
@@ -2645,7 +2645,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -2655,7 +2655,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="230">
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="237">
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241">
@@ -2795,7 +2795,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
@@ -2865,7 +2865,7 @@
         </is>
       </c>
       <c r="B250" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251">
@@ -2895,10 +2895,10 @@
         </is>
       </c>
       <c r="B253" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>